<commit_message>
Fixed command "examine chest"
Still doesn't move the instance to the inventory, but will display
correct info.
</commit_message>
<xml_diff>
--- a/dungeon_objects.xlsx
+++ b/dungeon_objects.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>name</t>
   </si>
@@ -616,7 +616,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +860,9 @@
       </c>
       <c r="M6" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>